<commit_message>
added 300uL pipette data
</commit_message>
<xml_diff>
--- a/data/commerical-Vs-printed-comparison/data-taking-raw/commercial-pipette-data-160127.xlsx
+++ b/data/commerical-Vs-printed-comparison/data-taking-raw/commercial-pipette-data-160127.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="0" windowWidth="23240" windowHeight="14300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Ependorf 200, 50, 20 uL" sheetId="2" r:id="rId1"/>
     <sheet name="Fisherbrand 10uL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -487,7 +492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -499,14 +504,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -550,7 +555,7 @@
         <v>198.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -572,7 +577,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -594,7 +599,7 @@
         <v>197.4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -616,7 +621,7 @@
         <v>197.1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -638,7 +643,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -663,7 +668,7 @@
         <v>196.32</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -673,7 +678,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -717,7 +722,7 @@
         <v>45.4</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -739,7 +744,7 @@
         <v>48.3</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -761,7 +766,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -783,7 +788,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -806,7 +811,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -831,7 +836,7 @@
         <v>47.879999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -841,7 +846,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,7 +868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -885,7 +890,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -907,7 +912,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -929,7 +934,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -951,7 +956,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -973,7 +978,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1015,14 +1020,14 @@
       <selection activeCell="I1" sqref="I1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1088,7 +1093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1110,7 +1115,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1132,7 +1137,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1154,7 +1159,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>